<commit_message>
increase to up to 5 source plates
</commit_message>
<xml_diff>
--- a/2-Inoculation/Inoculation_cherrypicking/input_inoculation_cherrypicking.xlsx
+++ b/2-Inoculation/Inoculation_cherrypicking/input_inoculation_cherrypicking.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bnortonb/Documents/Plate_Expressions_Purifications/2023-08-28-Example_folder/2-Inoculation/Inoculation_cherrypicking/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bnortonb/Documents/Automation_paper/opentrons/2-Inoculation/Inoculation_cherrypicking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4D2E26-58CD-5841-9BEF-B3637C644854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA857A04-200B-A043-B868-1F0A4D6DB4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35240" yWindow="1340" windowWidth="27640" windowHeight="16940" xr2:uid="{6D768310-9961-F147-832E-65DB87B0AFFA}"/>
+    <workbookView xWindow="16720" yWindow="880" windowWidth="19280" windowHeight="21320" xr2:uid="{6D768310-9961-F147-832E-65DB87B0AFFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="104">
   <si>
     <t>F10</t>
   </si>
@@ -342,13 +342,19 @@
   </si>
   <si>
     <t>sourceplate3</t>
+  </si>
+  <si>
+    <t>sourceplate4</t>
+  </si>
+  <si>
+    <t>sourceplate5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -360,14 +366,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -411,12 +409,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -436,9 +433,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -476,7 +473,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -582,7 +579,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -724,7 +721,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -734,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A2EBF6-38FB-994A-98D7-8993DF9530F3}">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,10 +742,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -759,8 +756,8 @@
       <c r="A2" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>96</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>89</v>
@@ -770,8 +767,8 @@
       <c r="A3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
+      <c r="B3" t="s">
+        <v>96</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>78</v>
@@ -781,8 +778,8 @@
       <c r="A4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>2</v>
+      <c r="B4" t="s">
+        <v>96</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>49</v>
@@ -792,8 +789,8 @@
       <c r="A5" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
+      <c r="B5" t="s">
+        <v>96</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>96</v>
@@ -803,8 +800,8 @@
       <c r="A6" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
+      <c r="B6" t="s">
+        <v>96</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>82</v>
@@ -814,8 +811,8 @@
       <c r="A7" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>5</v>
+      <c r="B7" t="s">
+        <v>96</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
@@ -825,8 +822,8 @@
       <c r="A8" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>6</v>
+      <c r="B8" t="s">
+        <v>96</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>33</v>
@@ -836,8 +833,8 @@
       <c r="A9" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>7</v>
+      <c r="B9" t="s">
+        <v>96</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -847,8 +844,8 @@
       <c r="A10" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
+      <c r="B10" t="s">
+        <v>96</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>43</v>
@@ -858,8 +855,8 @@
       <c r="A11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
+      <c r="B11" t="s">
+        <v>96</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>34</v>
@@ -869,8 +866,8 @@
       <c r="A12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
+      <c r="B12" t="s">
+        <v>96</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>52</v>
@@ -880,8 +877,8 @@
       <c r="A13" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>11</v>
+      <c r="B13" t="s">
+        <v>96</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>30</v>
@@ -891,8 +888,8 @@
       <c r="A14" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>12</v>
+      <c r="B14" t="s">
+        <v>82</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>41</v>
@@ -902,8 +899,8 @@
       <c r="A15" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>13</v>
+      <c r="B15" t="s">
+        <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>28</v>
@@ -913,8 +910,8 @@
       <c r="A16" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>14</v>
+      <c r="B16" t="s">
+        <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>48</v>
@@ -924,8 +921,8 @@
       <c r="A17" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>15</v>
+      <c r="B17" t="s">
+        <v>67</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>40</v>
@@ -935,8 +932,8 @@
       <c r="A18" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>24</v>
+      <c r="B18" t="s">
+        <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>85</v>
@@ -946,8 +943,8 @@
       <c r="A19" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>25</v>
+      <c r="B19" t="s">
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>75</v>
@@ -957,8 +954,8 @@
       <c r="A20" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>26</v>
+      <c r="B20" t="s">
+        <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>66</v>
@@ -968,8 +965,8 @@
       <c r="A21" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>27</v>
+      <c r="B21" t="s">
+        <v>56</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>14</v>
@@ -979,8 +976,8 @@
       <c r="A22" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>28</v>
+      <c r="B22" t="s">
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>63</v>
@@ -990,8 +987,8 @@
       <c r="A23" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>29</v>
+      <c r="B23" t="s">
+        <v>31</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>16</v>
@@ -1001,8 +998,8 @@
       <c r="A24" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>30</v>
+      <c r="B24" t="s">
+        <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>39</v>
@@ -1012,8 +1009,8 @@
       <c r="A25" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>91</v>
+      <c r="B25" t="s">
+        <v>88</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>91</v>
@@ -1023,8 +1020,8 @@
       <c r="A26" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>31</v>
+      <c r="B26" t="s">
+        <v>88</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>27</v>
@@ -1034,8 +1031,8 @@
       <c r="A27" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>32</v>
+      <c r="B27" t="s">
+        <v>88</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>42</v>
@@ -1045,8 +1042,8 @@
       <c r="A28" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>33</v>
+      <c r="B28" t="s">
+        <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>38</v>
@@ -1054,10 +1051,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>34</v>
+        <v>99</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>86</v>
@@ -1065,10 +1062,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>16</v>
+        <v>99</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>84</v>
@@ -1076,10 +1073,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>35</v>
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>62</v>
@@ -1089,8 +1086,8 @@
       <c r="A32" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>36</v>
+      <c r="B32" t="s">
+        <v>76</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>12</v>
@@ -1100,8 +1097,8 @@
       <c r="A33" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>37</v>
+      <c r="B33" t="s">
+        <v>79</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>53</v>
@@ -1111,8 +1108,8 @@
       <c r="A34" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>38</v>
+      <c r="B34" t="s">
+        <v>79</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>87</v>
@@ -1122,8 +1119,8 @@
       <c r="A35" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>39</v>
+      <c r="B35" t="s">
+        <v>45</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>47</v>
@@ -1133,8 +1130,8 @@
       <c r="A36" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>40</v>
+      <c r="B36" t="s">
+        <v>45</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>59</v>
@@ -1144,8 +1141,8 @@
       <c r="A37" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>41</v>
+      <c r="B37" t="s">
+        <v>45</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>54</v>
@@ -1155,8 +1152,8 @@
       <c r="A38" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>42</v>
+      <c r="B38" t="s">
+        <v>45</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>2</v>
@@ -1164,10 +1161,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>43</v>
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>32</v>
@@ -1175,10 +1172,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>44</v>
+        <v>101</v>
+      </c>
+      <c r="B40" t="s">
+        <v>89</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>97</v>
@@ -1186,10 +1183,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>45</v>
+        <v>101</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>25</v>
@@ -1197,10 +1194,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>46</v>
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>68</v>
@@ -1208,10 +1205,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>47</v>
+        <v>101</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>67</v>
@@ -1219,10 +1216,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>48</v>
+        <v>101</v>
+      </c>
+      <c r="B44" t="s">
+        <v>41</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>11</v>
@@ -1230,10 +1227,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>49</v>
+        <v>101</v>
+      </c>
+      <c r="B45" t="s">
+        <v>41</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>6</v>
@@ -1241,10 +1238,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>50</v>
+        <v>101</v>
+      </c>
+      <c r="B46" t="s">
+        <v>41</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>35</v>
@@ -1252,10 +1249,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>51</v>
+        <v>101</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>51</v>
@@ -1263,10 +1260,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>52</v>
+        <v>101</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>1</v>
@@ -1274,10 +1271,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>53</v>
+        <v>101</v>
+      </c>
+      <c r="B49" t="s">
+        <v>69</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>65</v>
@@ -1285,10 +1282,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>54</v>
+        <v>101</v>
+      </c>
+      <c r="B50" t="s">
+        <v>69</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>69</v>
@@ -1296,10 +1293,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>55</v>
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>60</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>60</v>
@@ -1307,10 +1304,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>56</v>
+        <v>101</v>
+      </c>
+      <c r="B52" t="s">
+        <v>60</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>74</v>
@@ -1318,10 +1315,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>57</v>
+        <v>101</v>
+      </c>
+      <c r="B53" t="s">
+        <v>60</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>7</v>
@@ -1329,10 +1326,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>58</v>
+        <v>101</v>
+      </c>
+      <c r="B54" t="s">
+        <v>60</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>20</v>
@@ -1340,10 +1337,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>59</v>
+        <v>101</v>
+      </c>
+      <c r="B55" t="s">
+        <v>60</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>81</v>
@@ -1351,9 +1348,9 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B56" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" t="s">
         <v>60</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -1362,10 +1359,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>61</v>
+        <v>101</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>46</v>
@@ -1373,10 +1370,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>62</v>
+        <v>101</v>
+      </c>
+      <c r="B58" t="s">
+        <v>22</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>26</v>
@@ -1384,10 +1381,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>63</v>
+        <v>101</v>
+      </c>
+      <c r="B59" t="s">
+        <v>57</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>37</v>
@@ -1395,10 +1392,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>64</v>
+        <v>101</v>
+      </c>
+      <c r="B60" t="s">
+        <v>57</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>58</v>
@@ -1406,10 +1403,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>65</v>
+        <v>102</v>
+      </c>
+      <c r="B61" t="s">
+        <v>96</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>50</v>
@@ -1417,10 +1414,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>66</v>
+        <v>102</v>
+      </c>
+      <c r="B62" t="s">
+        <v>96</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>61</v>
@@ -1428,10 +1425,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>67</v>
+        <v>102</v>
+      </c>
+      <c r="B63" t="s">
+        <v>96</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>29</v>
@@ -1439,10 +1436,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>68</v>
+        <v>102</v>
+      </c>
+      <c r="B64" t="s">
+        <v>96</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>44</v>
@@ -1450,10 +1447,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>69</v>
+        <v>102</v>
+      </c>
+      <c r="B65" t="s">
+        <v>10</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>76</v>
@@ -1461,10 +1458,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>70</v>
+        <v>102</v>
+      </c>
+      <c r="B66" t="s">
+        <v>10</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>22</v>
@@ -1472,10 +1469,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>16</v>
+        <v>102</v>
+      </c>
+      <c r="B67" t="s">
+        <v>10</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>73</v>
@@ -1483,10 +1480,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>12</v>
+        <v>102</v>
+      </c>
+      <c r="B68" t="s">
+        <v>10</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>90</v>
@@ -1494,10 +1491,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>17</v>
+        <v>102</v>
+      </c>
+      <c r="B69" t="s">
+        <v>40</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>4</v>
@@ -1505,10 +1502,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>18</v>
+        <v>102</v>
+      </c>
+      <c r="B70" t="s">
+        <v>40</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>98</v>
@@ -1516,10 +1513,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>19</v>
+        <v>102</v>
+      </c>
+      <c r="B71" t="s">
+        <v>12</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>0</v>
@@ -1527,10 +1524,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>20</v>
+        <v>102</v>
+      </c>
+      <c r="B72" t="s">
+        <v>12</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>80</v>
@@ -1538,10 +1535,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>4</v>
+        <v>102</v>
+      </c>
+      <c r="B73" t="s">
+        <v>12</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>15</v>
@@ -1549,10 +1546,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>21</v>
+        <v>102</v>
+      </c>
+      <c r="B74" t="s">
+        <v>12</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>3</v>
@@ -1560,10 +1557,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>22</v>
+        <v>102</v>
+      </c>
+      <c r="B75" t="s">
+        <v>12</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>9</v>
@@ -1571,10 +1568,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>13</v>
+        <v>102</v>
+      </c>
+      <c r="B76" t="s">
+        <v>67</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>24</v>
@@ -1582,10 +1579,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>23</v>
+        <v>102</v>
+      </c>
+      <c r="B77" t="s">
+        <v>67</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>55</v>
@@ -1593,10 +1590,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>79</v>
+        <v>102</v>
+      </c>
+      <c r="B78" t="s">
+        <v>67</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>21</v>
@@ -1604,10 +1601,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>68</v>
+        <v>102</v>
+      </c>
+      <c r="B79" t="s">
+        <v>37</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>71</v>
@@ -1615,10 +1612,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>90</v>
+        <v>102</v>
+      </c>
+      <c r="B80" t="s">
+        <v>37</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>57</v>
@@ -1626,10 +1623,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>35</v>
+        <v>102</v>
+      </c>
+      <c r="B81" t="s">
+        <v>37</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>8</v>
@@ -1637,10 +1634,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>81</v>
+        <v>102</v>
+      </c>
+      <c r="B82" t="s">
+        <v>37</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>79</v>
@@ -1648,10 +1645,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>43</v>
+        <v>102</v>
+      </c>
+      <c r="B83" t="s">
+        <v>37</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>13</v>
@@ -1659,10 +1656,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>77</v>
+        <v>102</v>
+      </c>
+      <c r="B84" t="s">
+        <v>37</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>56</v>
@@ -1670,10 +1667,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>11</v>
+        <v>102</v>
+      </c>
+      <c r="B85" t="s">
+        <v>37</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>70</v>
@@ -1681,10 +1678,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>47</v>
+        <v>102</v>
+      </c>
+      <c r="B86" t="s">
+        <v>37</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>36</v>
@@ -1692,10 +1689,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>8</v>
+        <v>102</v>
+      </c>
+      <c r="B87" t="s">
+        <v>58</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>45</v>
@@ -1703,10 +1700,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>91</v>
+        <v>103</v>
+      </c>
+      <c r="B88" t="s">
+        <v>58</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>31</v>
@@ -1714,10 +1711,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>51</v>
+        <v>103</v>
+      </c>
+      <c r="B89" t="s">
+        <v>77</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>5</v>
@@ -1725,10 +1722,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>37</v>
+        <v>103</v>
+      </c>
+      <c r="B90" t="s">
+        <v>77</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>88</v>
@@ -1736,10 +1733,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>75</v>
+        <v>103</v>
+      </c>
+      <c r="B91" t="s">
+        <v>77</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>83</v>
@@ -1747,10 +1744,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>46</v>
+        <v>103</v>
+      </c>
+      <c r="B92" t="s">
+        <v>77</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>19</v>
@@ -1758,10 +1755,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>71</v>
+        <v>103</v>
+      </c>
+      <c r="B93" t="s">
+        <v>77</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>72</v>
@@ -1769,10 +1766,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>57</v>
+        <v>103</v>
+      </c>
+      <c r="B94" t="s">
+        <v>77</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>92</v>
@@ -1780,10 +1777,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>63</v>
+        <v>103</v>
+      </c>
+      <c r="B95" t="s">
+        <v>77</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>23</v>
@@ -1791,10 +1788,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>67</v>
+        <v>103</v>
+      </c>
+      <c r="B96" t="s">
+        <v>77</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>64</v>
@@ -1802,17 +1799,17 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>56</v>
+        <v>103</v>
+      </c>
+      <c r="B97" t="s">
+        <v>77</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>